<commit_message>
Some test cases added
</commit_message>
<xml_diff>
--- a/TestCaseTemplateRBSU.xlsx
+++ b/TestCaseTemplateRBSU.xlsx
@@ -12,14 +12,18 @@
     <workbookView xWindow="0" yWindow="255" windowWidth="19065" windowHeight="8205"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Test User Account Viewing" sheetId="7" r:id="rId1"/>
+    <sheet name="Test Article Editing" sheetId="6" r:id="rId2"/>
+    <sheet name="Test Article Deleting" sheetId="5" r:id="rId3"/>
+    <sheet name="Test Article Publish" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="64">
   <si>
     <t>Expected Result</t>
   </si>
@@ -60,6 +64,9 @@
     <t>Articles</t>
   </si>
   <si>
+    <t>TC00001</t>
+  </si>
+  <si>
     <t>Expected result</t>
   </si>
   <si>
@@ -88,6 +95,126 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>Test article publish</t>
+  </si>
+  <si>
+    <t>Log in as site admin</t>
+  </si>
+  <si>
+    <t>Admin is still logged in</t>
+  </si>
+  <si>
+    <t>New article is uploaded</t>
+  </si>
+  <si>
+    <t>Open article options</t>
+  </si>
+  <si>
+    <t>Article options page is displayed</t>
+  </si>
+  <si>
+    <t>Click the new article button</t>
+  </si>
+  <si>
+    <t>Article editing page is displayed</t>
+  </si>
+  <si>
+    <t>Write article headline</t>
+  </si>
+  <si>
+    <t>Click post article button</t>
+  </si>
+  <si>
+    <t>New article is published and displayed at main page</t>
+  </si>
+  <si>
+    <t>Test article delete</t>
+  </si>
+  <si>
+    <t>Article is deleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Click the delete article option</t>
+  </si>
+  <si>
+    <t>Check if article exists</t>
+  </si>
+  <si>
+    <t>Article should not exist</t>
+  </si>
+  <si>
+    <t>TC00002</t>
+  </si>
+  <si>
+    <t>TC00003</t>
+  </si>
+  <si>
+    <t>Test article editing</t>
+  </si>
+  <si>
+    <t>Check article deletion functionality</t>
+  </si>
+  <si>
+    <t>Check article publishing functionality</t>
+  </si>
+  <si>
+    <t>Check article editing functionality</t>
+  </si>
+  <si>
+    <t>Article is edited</t>
+  </si>
+  <si>
+    <t>Click the edit article option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write article </t>
+  </si>
+  <si>
+    <t>Write new article headline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write new article </t>
+  </si>
+  <si>
+    <t>Article headline and content should be different</t>
+  </si>
+  <si>
+    <t>Test User Account Viewing</t>
+  </si>
+  <si>
+    <t>Test if you can view any user accounts as an admin</t>
+  </si>
+  <si>
+    <t>Must be logged in as admin</t>
+  </si>
+  <si>
+    <t>Admin still logged in</t>
+  </si>
+  <si>
+    <t>Open a users account</t>
+  </si>
+  <si>
+    <t>Open users menu in admin panel</t>
+  </si>
+  <si>
+    <t>Users page should be displaed</t>
+  </si>
+  <si>
+    <t>Find a user whos profile you whish to see</t>
+  </si>
+  <si>
+    <t>Click the account button on the right</t>
+  </si>
+  <si>
+    <t>User page should be shown</t>
+  </si>
+  <si>
+    <t>TC00005</t>
   </si>
 </sst>
 </file>
@@ -256,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -297,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +734,1096 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5">
+        <v>42476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>3</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5">
+        <v>42476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>3</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>4</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>5</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5">
+        <v>42476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>3</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5">
+        <v>42476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>3</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>4</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>5</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -672,19 +1891,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="15"/>
     </row>
@@ -694,25 +1913,25 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="15"/>
     </row>
@@ -722,22 +1941,22 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>0</v>

</xml_diff>